<commit_message>
fixed distance travelled computation
</commit_message>
<xml_diff>
--- a/HillShadeCalcs1.xlsx
+++ b/HillShadeCalcs1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Depth</t>
   </si>
@@ -33,6 +33,30 @@
   </si>
   <si>
     <t>GoodShade</t>
+  </si>
+  <si>
+    <t>SwathWidth</t>
+  </si>
+  <si>
+    <t>distanceTravelled</t>
+  </si>
+  <si>
+    <t>beams</t>
+  </si>
+  <si>
+    <t>myxres</t>
+  </si>
+  <si>
+    <t>Mean xRes</t>
+  </si>
+  <si>
+    <t>npings</t>
+  </si>
+  <si>
+    <t>myyres</t>
+  </si>
+  <si>
+    <t>Mean yRes</t>
   </si>
 </sst>
 </file>
@@ -352,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="344064520"/>
-        <c:axId val="344058248"/>
+        <c:axId val="245576600"/>
+        <c:axId val="245578560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="344064520"/>
+        <c:axId val="245576600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,12 +493,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344058248"/>
+        <c:crossAx val="245578560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="344058248"/>
+        <c:axId val="245578560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +611,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344064520"/>
+        <c:crossAx val="245576600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -896,11 +920,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404076872"/>
-        <c:axId val="404076480"/>
+        <c:axId val="245573072"/>
+        <c:axId val="245579344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404076872"/>
+        <c:axId val="245573072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,12 +981,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404076480"/>
+        <c:crossAx val="245579344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404076480"/>
+        <c:axId val="245579344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404076872"/>
+        <c:crossAx val="245573072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2508,15 +2532,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2527,7 +2554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5.58</v>
       </c>
@@ -2538,7 +2565,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>32</v>
       </c>
@@ -2549,7 +2576,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>35</v>
       </c>
@@ -2560,7 +2587,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>37</v>
       </c>
@@ -2571,7 +2598,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>91</v>
       </c>
@@ -2582,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>236</v>
       </c>
@@ -2593,7 +2620,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1728</v>
       </c>
@@ -2604,7 +2631,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2767</v>
       </c>
@@ -2615,7 +2642,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2758</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2973</v>
       </c>
@@ -2637,7 +2664,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3684</v>
       </c>
@@ -2646,6 +2673,72 @@
       </c>
       <c r="C12">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>58.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <f>B23/B24</f>
+        <v>0.14527499999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>257.43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <f>B29/B30</f>
+        <v>0.21049059689288635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>